<commit_message>
refactored model and repo
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReportTeam.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReportTeam.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VVSS\02_Inventory\Docs\Lab01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96220E8F-793B-4892-B78F-CB24420AFA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496" tabRatio="650" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -12,25 +18,12 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -532,12 +525,252 @@
   <si>
     <t>AddProductController/121</t>
   </si>
+  <si>
+    <t>Product product = new Product(0, null, 0.0, 0, 0, 0, null);
+            return product;</t>
+  </si>
+  <si>
+    <t>Unnecessary variable used. Could be returned directly</t>
+  </si>
+  <si>
+    <t>Inventory/50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> return new Product(0, null, 0.0, 0, 0, 0, null);</t>
+  </si>
+  <si>
+    <t>Inventory/49</t>
+  </si>
+  <si>
+    <t>unnecessary boolean literal</t>
+  </si>
+  <si>
+    <t>if(isFound == false)</t>
+  </si>
+  <si>
+    <t>if(!isFound)</t>
+  </si>
+  <si>
+    <t>Part/16</t>
+  </si>
+  <si>
+    <t>The constructor can be made protected.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC66D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Part</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>partId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>String name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, double </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>inStock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">max) </t>
+    </r>
+  </si>
+  <si>
+    <t>protected Part(int partId, String name, double price, int inStock, int min, int max)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> associatedParts = associatedParts</t>
+  </si>
+  <si>
+    <t>there is a confusion. If the left hand part is a class field should be referenced with "this"</t>
+  </si>
+  <si>
+    <t>this.associatedParts = associatedParts;</t>
+  </si>
+  <si>
+    <t>Product/60</t>
+  </si>
+  <si>
+    <t>import javafx.collections.FXCollections;</t>
+  </si>
+  <si>
+    <t>the import is unused</t>
+  </si>
+  <si>
+    <t>Product/4</t>
+  </si>
+  <si>
+    <t>InventoryRepository/148</t>
+  </si>
+  <si>
+    <t>line=line+list.get(index).getPartId()+":";</t>
+  </si>
+  <si>
+    <t>is preffered to use a StringBuilder instead of concatenation</t>
+  </si>
+  <si>
+    <t>line.append(list.get(index).getPartId()).append(":");</t>
+  </si>
+  <si>
+    <t>InventoryRepository/35</t>
+  </si>
+  <si>
+    <t>catch (FileNotFoundException e) {
+   e.printStackTrace();
+  } catch (IOException e) {
+   e.printStackTrace();
+  }</t>
+  </si>
+  <si>
+    <t>2 catches doing the exactly same thing. Can be combined in a single one</t>
+  </si>
+  <si>
+    <t>catch (IOException e) {
+   e.printStackTrace();</t>
+  </si>
+  <si>
+    <t>Bufferreader wont be closed if exceptions occur. Either try with resources or being closed in finally should be implemented</t>
+  </si>
+  <si>
+    <t>try {
+   br = new BufferedReader(new FileReader(file)); …</t>
+  </si>
+  <si>
+    <t>try (BufferedReader br = new BufferedReader(new FileReader(file))) {</t>
+  </si>
+  <si>
+    <t>InventoryRepository/75</t>
+  </si>
+  <si>
+    <t>System.out.println(p.toString());</t>
+  </si>
+  <si>
+    <t>System.out.println can be replaced by a logger</t>
+  </si>
+  <si>
+    <t>logger.info(p);</t>
+  </si>
+  <si>
+    <t>InventoryRepository/124</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,6 +898,24 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCC7832"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC66D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -765,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -796,6 +1047,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -838,20 +1104,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,7 +1125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -913,7 +1167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -946,9 +1200,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -981,6 +1252,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1156,7 +1444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1183,19 +1471,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1215,10 +1503,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1229,10 +1517,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1244,15 +1532,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1465,13 +1753,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1491,19 +1779,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1523,10 +1811,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1537,10 +1825,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1552,15 +1840,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1772,7 +2060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1799,19 +2087,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1831,10 +2119,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1845,10 +2133,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="38"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1860,15 +2148,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -2120,14 +2408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2135,8 +2423,8 @@
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
     <col min="3" max="3" width="22.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
@@ -2148,19 +2436,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2180,8 +2468,8 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2192,8 +2480,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2205,8 +2493,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10">
@@ -2253,10 +2541,10 @@
       <c r="D11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="26" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2270,10 +2558,10 @@
       <c r="D12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="23" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2288,7 +2576,7 @@
       <c r="D13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="24" t="s">
         <v>77</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -2309,7 +2597,7 @@
       <c r="E14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="25" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2324,14 +2612,14 @@
       <c r="D15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="25" t="s">
         <v>83</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.8">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2414,7 +2702,7 @@
       <c r="D20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="25" t="s">
         <v>108</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -2439,95 +2727,167 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" ht="28.8">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="2:6">
+      <c r="C23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="28.8">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="2:6">
+      <c r="C24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="28.8">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="2:6">
+      <c r="C27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="72">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="2:6">
+      <c r="C28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="43.2">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="3">
@@ -2540,11 +2900,11 @@
       <c r="F31" s="2"/>
     </row>
     <row r="33" spans="3:6">
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
       <c r="F33" s="18"/>
     </row>
     <row r="36" spans="3:6">

</xml_diff>